<commit_message>
Handle updating DeTai when GiangVien is Updated
</commit_message>
<xml_diff>
--- a/server/giangViens.xlsx
+++ b/server/giangViens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\QuanLyKhoaLuan\quan-ly-khoa-luan\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A71403-F1F0-47C7-9577-8201B8DDAE09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA5FF33-6C29-4A50-A8FE-7A4BEB222517}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Trần Văn A</t>
-  </si>
-  <si>
     <t>Trần Văn B</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Trần Văn D</t>
   </si>
   <si>
-    <t>Trần Văn E</t>
-  </si>
-  <si>
     <t>ThS.</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>etv@uit.edu.vn</t>
+  </si>
+  <si>
+    <t>Trần Văn Eii</t>
+  </si>
+  <si>
+    <t>Trần Văn Aii.</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,19 +504,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -524,19 +524,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -544,19 +544,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -564,19 +564,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -584,19 +584,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>